<commit_message>
mlk holiday jan added
</commit_message>
<xml_diff>
--- a/2023_cboc_signin_sheets/01January_2023_cboc_signin_sheet.xlsx
+++ b/2023_cboc_signin_sheets/01January_2023_cboc_signin_sheet.xlsx
@@ -2748,8 +2748,8 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col customWidth="1" max="1" min="1" width="12.5"/>
-    <col customWidth="1" max="2" min="2" width="4.5"/>
-    <col customWidth="1" max="3" min="3" width="4.5"/>
+    <col customWidth="1" max="2" min="2" width="2.5"/>
+    <col customWidth="1" max="3" min="3" width="2.5"/>
     <col customWidth="1" max="4" min="4" width="4.5"/>
     <col customWidth="1" max="5" min="5" width="4.5"/>
     <col customWidth="1" max="6" min="6" width="4.5"/>
@@ -2827,12 +2827,12 @@
           <t>CBOC/CORE</t>
         </is>
       </c>
-      <c r="B2" s="7" t="inlineStr">
+      <c r="B2" s="5" t="inlineStr">
         <is>
           <t>MON</t>
         </is>
       </c>
-      <c r="C2" s="8" t="n"/>
+      <c r="C2" s="6" t="n"/>
       <c r="D2" s="7" t="inlineStr">
         <is>
           <t>TUE</t>
@@ -2930,10 +2930,10 @@
           <t>Date</t>
         </is>
       </c>
-      <c r="B3" s="7" t="n">
+      <c r="B3" s="5" t="n">
         <v>16</v>
       </c>
-      <c r="C3" s="8" t="n"/>
+      <c r="C3" s="6" t="n"/>
       <c r="D3" s="7" t="n">
         <v>17</v>
       </c>
@@ -2997,12 +2997,12 @@
     </row>
     <row customHeight="1" ht="27" r="4">
       <c r="A4" s="10" t="n"/>
-      <c r="B4" s="13" t="inlineStr">
+      <c r="B4" s="11" t="inlineStr">
         <is>
           <t>Tech</t>
         </is>
       </c>
-      <c r="C4" s="14" t="inlineStr">
+      <c r="C4" s="12" t="inlineStr">
         <is>
           <t>Time of Arrival</t>
         </is>
@@ -3164,8 +3164,16 @@
           <t>Oak Lawn</t>
         </is>
       </c>
-      <c r="B5" s="18" t="n"/>
-      <c r="C5" s="19" t="n"/>
+      <c r="B5" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C5" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D5" s="18" t="n"/>
       <c r="E5" s="19" t="n"/>
       <c r="F5" s="18" t="n"/>
@@ -3235,8 +3243,16 @@
           <t>Frozen</t>
         </is>
       </c>
-      <c r="B6" s="23" t="n"/>
-      <c r="C6" s="24" t="n"/>
+      <c r="B6" s="21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C6" s="22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D6" s="23" t="n"/>
       <c r="E6" s="24" t="n"/>
       <c r="F6" s="23" t="n"/>
@@ -3302,8 +3318,8 @@
     </row>
     <row customHeight="1" ht="10" r="7">
       <c r="A7" s="10" t="n"/>
-      <c r="B7" s="27" t="n"/>
-      <c r="C7" s="28" t="n"/>
+      <c r="B7" s="25" t="n"/>
+      <c r="C7" s="26" t="n"/>
       <c r="D7" s="27" t="n"/>
       <c r="E7" s="28" t="n"/>
       <c r="F7" s="27" t="n"/>
@@ -3341,8 +3357,16 @@
           <t>Hoffman Est.</t>
         </is>
       </c>
-      <c r="B8" s="18" t="n"/>
-      <c r="C8" s="19" t="n"/>
+      <c r="B8" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C8" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D8" s="18" t="n"/>
       <c r="E8" s="19" t="n"/>
       <c r="F8" s="18" t="n"/>
@@ -3412,8 +3436,16 @@
           <t>Frozen</t>
         </is>
       </c>
-      <c r="B9" s="23" t="n"/>
-      <c r="C9" s="24" t="n"/>
+      <c r="B9" s="21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C9" s="22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D9" s="23" t="n"/>
       <c r="E9" s="24" t="n"/>
       <c r="F9" s="23" t="n"/>
@@ -3479,8 +3511,8 @@
     </row>
     <row customHeight="1" ht="10" r="10">
       <c r="A10" s="10" t="n"/>
-      <c r="B10" s="27" t="n"/>
-      <c r="C10" s="28" t="n"/>
+      <c r="B10" s="25" t="n"/>
+      <c r="C10" s="26" t="n"/>
       <c r="D10" s="27" t="n"/>
       <c r="E10" s="28" t="n"/>
       <c r="F10" s="27" t="n"/>
@@ -3518,8 +3550,16 @@
           <t>Aurora</t>
         </is>
       </c>
-      <c r="B11" s="18" t="n"/>
-      <c r="C11" s="19" t="n"/>
+      <c r="B11" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C11" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D11" s="18" t="n"/>
       <c r="E11" s="19" t="n"/>
       <c r="F11" s="18" t="n"/>
@@ -3589,8 +3629,16 @@
           <t>Frozen</t>
         </is>
       </c>
-      <c r="B12" s="23" t="n"/>
-      <c r="C12" s="24" t="n"/>
+      <c r="B12" s="21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C12" s="22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D12" s="23" t="n"/>
       <c r="E12" s="24" t="n"/>
       <c r="F12" s="23" t="n"/>
@@ -3656,8 +3704,8 @@
     </row>
     <row customHeight="1" ht="10" r="13">
       <c r="A13" s="10" t="n"/>
-      <c r="B13" s="27" t="n"/>
-      <c r="C13" s="28" t="n"/>
+      <c r="B13" s="25" t="n"/>
+      <c r="C13" s="26" t="n"/>
       <c r="D13" s="27" t="n"/>
       <c r="E13" s="28" t="n"/>
       <c r="F13" s="27" t="n"/>
@@ -3695,8 +3743,16 @@
           <t>Kankakee</t>
         </is>
       </c>
-      <c r="B14" s="18" t="n"/>
-      <c r="C14" s="19" t="n"/>
+      <c r="B14" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C14" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D14" s="18" t="n"/>
       <c r="E14" s="19" t="n"/>
       <c r="F14" s="18" t="n"/>
@@ -3766,8 +3822,16 @@
           <t>Frozen</t>
         </is>
       </c>
-      <c r="B15" s="23" t="n"/>
-      <c r="C15" s="24" t="n"/>
+      <c r="B15" s="21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C15" s="22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D15" s="23" t="n"/>
       <c r="E15" s="24" t="n"/>
       <c r="F15" s="23" t="n"/>
@@ -3833,8 +3897,8 @@
     </row>
     <row customHeight="1" ht="10" r="16">
       <c r="A16" s="10" t="n"/>
-      <c r="B16" s="27" t="n"/>
-      <c r="C16" s="28" t="n"/>
+      <c r="B16" s="25" t="n"/>
+      <c r="C16" s="26" t="n"/>
       <c r="D16" s="27" t="n"/>
       <c r="E16" s="28" t="n"/>
       <c r="F16" s="27" t="n"/>
@@ -3872,8 +3936,16 @@
           <t>LaSalle</t>
         </is>
       </c>
-      <c r="B17" s="18" t="n"/>
-      <c r="C17" s="19" t="n"/>
+      <c r="B17" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C17" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D17" s="18" t="n"/>
       <c r="E17" s="19" t="n"/>
       <c r="F17" s="18" t="n"/>
@@ -3943,8 +4015,16 @@
           <t>Frozen</t>
         </is>
       </c>
-      <c r="B18" s="23" t="n"/>
-      <c r="C18" s="24" t="n"/>
+      <c r="B18" s="21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C18" s="22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D18" s="23" t="n"/>
       <c r="E18" s="24" t="n"/>
       <c r="F18" s="23" t="n"/>
@@ -4010,8 +4090,8 @@
     </row>
     <row customHeight="1" ht="10" r="19">
       <c r="A19" s="10" t="n"/>
-      <c r="B19" s="27" t="n"/>
-      <c r="C19" s="28" t="n"/>
+      <c r="B19" s="25" t="n"/>
+      <c r="C19" s="26" t="n"/>
       <c r="D19" s="27" t="n"/>
       <c r="E19" s="28" t="n"/>
       <c r="F19" s="27" t="n"/>
@@ -4049,8 +4129,16 @@
           <t>Joliet</t>
         </is>
       </c>
-      <c r="B20" s="18" t="n"/>
-      <c r="C20" s="19" t="n"/>
+      <c r="B20" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C20" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D20" s="18" t="n"/>
       <c r="E20" s="19" t="n"/>
       <c r="F20" s="18" t="n"/>
@@ -4120,8 +4208,16 @@
           <t>Frozen</t>
         </is>
       </c>
-      <c r="B21" s="23" t="n"/>
-      <c r="C21" s="24" t="n"/>
+      <c r="B21" s="21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C21" s="22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D21" s="23" t="n"/>
       <c r="E21" s="24" t="n"/>
       <c r="F21" s="23" t="n"/>
@@ -4187,8 +4283,8 @@
     </row>
     <row customHeight="1" ht="10" r="22">
       <c r="A22" s="10" t="n"/>
-      <c r="B22" s="27" t="n"/>
-      <c r="C22" s="28" t="n"/>
+      <c r="B22" s="25" t="n"/>
+      <c r="C22" s="26" t="n"/>
       <c r="D22" s="27" t="n"/>
       <c r="E22" s="28" t="n"/>
       <c r="F22" s="27" t="n"/>
@@ -4226,8 +4322,16 @@
           <t>Jesse Brown</t>
         </is>
       </c>
-      <c r="B23" s="18" t="n"/>
-      <c r="C23" s="19" t="n"/>
+      <c r="B23" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C23" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D23" s="18" t="n"/>
       <c r="E23" s="19" t="n"/>
       <c r="F23" s="18" t="n"/>
@@ -4297,8 +4401,16 @@
           <t>Frozen</t>
         </is>
       </c>
-      <c r="B24" s="23" t="n"/>
-      <c r="C24" s="24" t="n"/>
+      <c r="B24" s="21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C24" s="22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D24" s="23" t="n"/>
       <c r="E24" s="24" t="n"/>
       <c r="F24" s="23" t="n"/>
@@ -4364,8 +4476,8 @@
     </row>
     <row customHeight="1" ht="10" r="25">
       <c r="A25" s="10" t="n"/>
-      <c r="B25" s="27" t="n"/>
-      <c r="C25" s="28" t="n"/>
+      <c r="B25" s="25" t="n"/>
+      <c r="C25" s="26" t="n"/>
       <c r="D25" s="27" t="n"/>
       <c r="E25" s="28" t="n"/>
       <c r="F25" s="27" t="n"/>
@@ -4403,8 +4515,16 @@
           <t>Crown Point</t>
         </is>
       </c>
-      <c r="B26" s="18" t="n"/>
-      <c r="C26" s="19" t="n"/>
+      <c r="B26" s="16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C26" s="17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D26" s="18" t="n"/>
       <c r="E26" s="19" t="n"/>
       <c r="F26" s="18" t="n"/>
@@ -4474,8 +4594,16 @@
           <t>Frozen</t>
         </is>
       </c>
-      <c r="B27" s="31" t="n"/>
-      <c r="C27" s="32" t="n"/>
+      <c r="B27" s="29" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C27" s="30" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D27" s="31" t="n"/>
       <c r="E27" s="32" t="n"/>
       <c r="F27" s="31" t="n"/>

</xml_diff>